<commit_message>
Update parcel registrations Simprints integration
</commit_message>
<xml_diff>
--- a/xlsx/form_p_parcels.xlsx
+++ b/xlsx/form_p_parcels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Terra_Share\projects\CaVaTeCo_Collect\projects\odk_forms_cesc_niassa\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811FE230-5FD7-402B-8B2A-A6186E900850}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B22A602-2416-4EE6-9160-7F3940B043C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -834,13 +834,7 @@
     <t>"jHcAAHvZzSjuAaQfT3pm"</t>
   </si>
   <si>
-    <t>http://cavateco.terrafirma.co.mz:8080/sandbox/submission</t>
-  </si>
-  <si>
     <t>selected_user_guid</t>
-  </si>
-  <si>
-    <t>if (${odk-tiers}='', '', if ((string-length(${odk-tiers})&gt;0 and ${odk-tiers}!= 'TIER_5'), 'FOI', 'NÃO FOI'))</t>
   </si>
   <si>
     <t>parties_number</t>
@@ -987,14 +981,27 @@
 &lt;h1&gt;&lt;span style="color:#57b055"&gt;${party_name}&lt;/span&gt; 
 &lt;h1&gt;&lt;span style="color:#FF6347"&gt;${verified}&lt;/span&gt; verificada</t>
   </si>
+  <si>
+    <t>http://cavateco.terrafirma.co.mz:8080/cesc_niassa/submission</t>
+  </si>
+  <si>
+    <t>if (${odk-confidences}='', '', if ((${odk-confidences}&gt;=55), 'FOI', 'NÃO FOI'))</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1397,563 +1404,563 @@
   </borders>
   <cellStyleXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="244"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="244" applyFill="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="244" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="244" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="244" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="0" xfId="244" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="244"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="244" applyFill="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="244" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="244" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="244" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="0" xfId="244" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="258" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="258" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="259">
@@ -2554,11 +2561,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,7 +2776,7 @@
         <v>103</v>
       </c>
       <c r="C13" s="129" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D13" s="101"/>
     </row>
@@ -3254,7 +3261,7 @@
         <v>107</v>
       </c>
       <c r="J38" s="132" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K38" s="27" t="s">
         <v>21</v>
@@ -3367,17 +3374,17 @@
         <v>26</v>
       </c>
       <c r="B45" s="110" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C45" s="120" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D45" s="86"/>
       <c r="I45" s="109" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J45" s="131" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K45" s="42" t="s">
         <v>21</v>
@@ -3388,14 +3395,14 @@
         <v>43</v>
       </c>
       <c r="B46" s="53" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D46" s="1"/>
       <c r="F46" s="109" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:13" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3406,7 +3413,7 @@
         <v>108</v>
       </c>
       <c r="C47" s="111" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D47" s="58"/>
       <c r="E47" s="86" t="s">
@@ -3426,7 +3433,7 @@
         <v>63</v>
       </c>
       <c r="C48" s="112" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D48" s="43"/>
       <c r="J48" s="131"/>
@@ -3442,11 +3449,11 @@
         <v>153</v>
       </c>
       <c r="C49" s="91" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D49" s="91"/>
       <c r="G49" s="117" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J49" s="131"/>
       <c r="K49" s="55" t="s">
@@ -3464,7 +3471,7 @@
         <v>66</v>
       </c>
       <c r="O50" s="109" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
@@ -3472,13 +3479,13 @@
         <v>35</v>
       </c>
       <c r="B51" s="108" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C51" s="93"/>
       <c r="D51" s="93"/>
       <c r="H51" s="55"/>
       <c r="O51" s="109" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:15" s="104" customFormat="1" x14ac:dyDescent="0.25">
@@ -3486,10 +3493,10 @@
         <v>35</v>
       </c>
       <c r="B52" s="130" t="s">
+        <v>295</v>
+      </c>
+      <c r="O52" s="131" t="s">
         <v>297</v>
-      </c>
-      <c r="O52" s="131" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="53" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
@@ -3497,13 +3504,13 @@
         <v>35</v>
       </c>
       <c r="B53" s="130" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C53" s="93"/>
       <c r="D53" s="93"/>
       <c r="H53" s="55"/>
       <c r="O53" s="131" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="54" spans="1:15" s="125" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3517,7 +3524,7 @@
         <v>245</v>
       </c>
       <c r="D54" s="55" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E54" s="124"/>
       <c r="M54" s="126" t="s">
@@ -3629,7 +3636,7 @@
       <c r="D63" s="55"/>
       <c r="H63" s="55"/>
       <c r="O63" s="126" t="s">
-        <v>267</v>
+        <v>302</v>
       </c>
     </row>
     <row r="64" spans="1:15" s="86" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3640,7 +3647,7 @@
         <v>263</v>
       </c>
       <c r="C64" s="135" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D64" s="43"/>
       <c r="H64" s="55"/>
@@ -3651,17 +3658,17 @@
         <v>224</v>
       </c>
       <c r="B65" s="128" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C65" s="134" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D65" s="88"/>
       <c r="G65" s="134" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H65" s="55" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I65" s="55"/>
       <c r="J65" s="131"/>
@@ -3697,7 +3704,7 @@
         <v>35</v>
       </c>
       <c r="B67" s="113" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C67" s="58"/>
       <c r="D67" s="58"/>
@@ -3705,7 +3712,7 @@
       <c r="H67" s="55"/>
       <c r="K67" s="63"/>
       <c r="O67" s="112" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
@@ -3718,10 +3725,10 @@
         <v>35</v>
       </c>
       <c r="B69" s="115" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="O69" s="112" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -3729,19 +3736,19 @@
         <v>224</v>
       </c>
       <c r="B70" s="130" t="s">
+        <v>286</v>
+      </c>
+      <c r="C70" s="133" t="s">
+        <v>294</v>
+      </c>
+      <c r="H70" s="114" t="s">
+        <v>280</v>
+      </c>
+      <c r="I70" s="114" t="s">
+        <v>279</v>
+      </c>
+      <c r="J70" s="131" t="s">
         <v>288</v>
-      </c>
-      <c r="C70" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="H70" s="114" t="s">
-        <v>282</v>
-      </c>
-      <c r="I70" s="114" t="s">
-        <v>281</v>
-      </c>
-      <c r="J70" s="131" t="s">
-        <v>290</v>
       </c>
       <c r="K70" s="131" t="s">
         <v>21</v>
@@ -3853,7 +3860,7 @@
         <v>46</v>
       </c>
       <c r="C77" s="134" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D77" s="30"/>
       <c r="J77" s="25"/>
@@ -9594,8 +9601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9636,7 +9643,7 @@
         <v>2021052713</v>
       </c>
       <c r="D2" s="98" t="s">
-        <v>265</v>
+        <v>301</v>
       </c>
       <c r="E2" s="66" t="s">
         <v>170</v>

</xml_diff>